<commit_message>
Version 15 Junio 2020
Versión de los archivos del 15 de junio 2020
</commit_message>
<xml_diff>
--- a/2020/Directivos-colegio/Coordinacion/listados/20200601 Listado de medios de comunicacion con estudiantes.xlsx
+++ b/2020/Directivos-colegio/Coordinacion/listados/20200601 Listado de medios de comunicacion con estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\Directivos-colegio\Coordinacion\listados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D584EDC7-1FB2-41F7-A02C-7E9881D1931A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412D848-A4CD-44B2-A9CF-1C96CF10C6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="555" windowWidth="14400" windowHeight="13710" tabRatio="710" firstSheet="1" activeTab="8" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="710" firstSheet="1" activeTab="2" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="532">
   <si>
     <t>Codigo</t>
   </si>
@@ -2906,10 +2906,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>27</c:v>
@@ -2921,13 +2921,13 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -3098,10 +3098,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>9</c:v>
@@ -3113,13 +3113,13 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>32</c:v>
@@ -3573,10 +3573,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.85</c:v>
+                  <c:v>0.875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.8823529411764705E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.75</c:v>
@@ -3588,13 +3588,13 @@
                   <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70588235294117652</c:v>
+                  <c:v>0.73529411764705888</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.82352941176470584</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9411764705882353E-2</c:v>
+                  <c:v>8.8235294117647065E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3.0303030303030304E-2</c:v>
@@ -3762,10 +3762,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0.15</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.25</c:v>
@@ -3777,13 +3777,13 @@
                   <c:v>0.29411764705882354</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.29411764705882354</c:v>
+                  <c:v>0.26470588235294118</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.17647058823529413</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.97058823529411764</c:v>
+                  <c:v>0.91176470588235292</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.96969696969696972</c:v>
@@ -5627,11 +5627,11 @@
       </c>
       <c r="B5" s="10">
         <f>'06-1'!D50</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="10">
         <f>'08-1'!D44</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="10">
         <f>'08-2'!D46</f>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="G5" s="10">
         <f>'09-1'!D44</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="10">
         <f>'09-2'!D44</f>
@@ -5655,7 +5655,7 @@
       </c>
       <c r="I5" s="10">
         <f>'09-3'!D44</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J5" s="10">
         <f>'10-1'!D43</f>
@@ -5683,11 +5683,11 @@
       </c>
       <c r="P5" s="33">
         <f t="shared" ref="P5:P8" si="0">AVERAGE(B5:O5)</f>
-        <v>11.928571428571429</v>
+        <v>12.357142857142858</v>
       </c>
       <c r="Q5" s="33">
         <f t="shared" ref="Q5:Q8" si="1">MAX(B5:O5)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="R5" s="33">
         <f t="shared" ref="R5:R8" si="2">MIN(B5:O5)</f>
@@ -5700,11 +5700,11 @@
       </c>
       <c r="B6" s="10">
         <f>'06-1'!D51</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="10">
         <f>'08-1'!D45</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D6" s="10">
         <f>'08-2'!D47</f>
@@ -5720,7 +5720,7 @@
       </c>
       <c r="G6" s="10">
         <f>'09-1'!D45</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" s="10">
         <f>'09-2'!D45</f>
@@ -5728,7 +5728,7 @@
       </c>
       <c r="I6" s="10">
         <f>'09-3'!D45</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6" s="10">
         <f>'10-1'!D44</f>
@@ -5756,7 +5756,7 @@
       </c>
       <c r="P6" s="33">
         <f t="shared" si="0"/>
-        <v>22.142857142857142</v>
+        <v>21.714285714285715</v>
       </c>
       <c r="Q6" s="33">
         <f t="shared" si="1"/>
@@ -5764,7 +5764,7 @@
       </c>
       <c r="R6" s="33">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5773,11 +5773,11 @@
       </c>
       <c r="B7" s="32">
         <f>B5/B4</f>
-        <v>0.85</v>
+        <v>0.875</v>
       </c>
       <c r="C7" s="32">
         <f t="shared" ref="C7:O7" si="3">C5/C4</f>
-        <v>0</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="D7" s="32">
         <f t="shared" si="3"/>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="G7" s="32">
         <f t="shared" si="3"/>
-        <v>0.70588235294117652</v>
+        <v>0.73529411764705888</v>
       </c>
       <c r="H7" s="32">
         <f t="shared" si="3"/>
@@ -5801,7 +5801,7 @@
       </c>
       <c r="I7" s="32">
         <f t="shared" si="3"/>
-        <v>2.9411764705882353E-2</v>
+        <v>8.8235294117647065E-2</v>
       </c>
       <c r="J7" s="32">
         <f t="shared" si="3"/>
@@ -5829,11 +5829,11 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0.33882098293863006</v>
+        <v>0.35111089890501651</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="1"/>
-        <v>0.85</v>
+        <v>0.875</v>
       </c>
       <c r="R7" s="34">
         <f t="shared" si="2"/>
@@ -5846,11 +5846,11 @@
       </c>
       <c r="B8" s="36">
         <f>B6/B4</f>
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="C8" s="36">
         <f t="shared" ref="C8:O8" si="4">C6/C4</f>
-        <v>1</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="D8" s="36">
         <f t="shared" si="4"/>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="G8" s="36">
         <f t="shared" si="4"/>
-        <v>0.29411764705882354</v>
+        <v>0.26470588235294118</v>
       </c>
       <c r="H8" s="36">
         <f t="shared" si="4"/>
@@ -5874,7 +5874,7 @@
       </c>
       <c r="I8" s="36">
         <f t="shared" si="4"/>
-        <v>0.97058823529411764</v>
+        <v>0.91176470588235292</v>
       </c>
       <c r="J8" s="36">
         <f t="shared" si="4"/>
@@ -5902,7 +5902,7 @@
       </c>
       <c r="P8" s="37">
         <f t="shared" si="0"/>
-        <v>0.66117901706137006</v>
+        <v>0.64888910109498354</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
@@ -5910,7 +5910,7 @@
       </c>
       <c r="R8" s="37">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -10253,8 +10253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D44"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10588,9 +10588,12 @@
       <c r="C18" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="I18" t="s">
         <v>43</v>
@@ -11132,7 +11135,7 @@
       <c r="C45" s="55"/>
       <c r="D45" s="22">
         <f>COUNTA(D5:D44)</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E45" s="22">
         <f t="shared" ref="E45:G45" si="1">COUNTA(E5:E44)</f>
@@ -11148,7 +11151,7 @@
       </c>
       <c r="H45" s="23">
         <f>COUNTIF(H5:H44,"X")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -11186,11 +11189,11 @@
       </c>
       <c r="D50" s="10">
         <f>D49-D51</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E50" s="12">
         <f>D50/$D$49</f>
-        <v>0.85</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="51" spans="3:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -11199,11 +11202,11 @@
       </c>
       <c r="D51" s="10">
         <f>H45</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E51" s="12">
         <f>D51/$D$49</f>
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>
@@ -11230,8 +11233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8FFEA4-FAE9-4E98-A7DA-1A249C6193F4}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11380,9 +11383,12 @@
       <c r="C10" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -11440,9 +11446,12 @@
       <c r="C14" s="9" t="s">
         <v>90</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -11813,7 +11822,7 @@
       <c r="C39" s="55"/>
       <c r="D39" s="22">
         <f>COUNTA(D5:D38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E39" s="22">
         <f t="shared" ref="E39:G39" si="1">COUNTA(E5:E38)</f>
@@ -11829,7 +11838,7 @@
       </c>
       <c r="H39" s="23">
         <f>COUNTIF(H5:H38,"X")</f>
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -11863,11 +11872,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -11876,11 +11885,11 @@
       </c>
       <c r="D45" s="10">
         <f>H39</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>1</v>
+        <v>0.94117647058823528</v>
       </c>
     </row>
   </sheetData>
@@ -14445,7 +14454,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14954,9 +14963,12 @@
       <c r="C30" s="9" t="s">
         <v>244</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -15111,7 +15123,7 @@
       <c r="C39" s="55"/>
       <c r="D39" s="22">
         <f>COUNTA(D5:D38)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E39" s="22">
         <f t="shared" ref="E39:G39" si="1">COUNTA(E5:E38)</f>
@@ -15127,7 +15139,7 @@
       </c>
       <c r="H39" s="23">
         <f>COUNTIF($H$5:$H$38,"X")</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -15161,11 +15173,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0.70588235294117652</v>
+        <v>0.73529411764705888</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -15174,11 +15186,11 @@
       </c>
       <c r="D45" s="10">
         <f>H39</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>0.29411764705882354</v>
+        <v>0.26470588235294118</v>
       </c>
     </row>
   </sheetData>
@@ -16081,8 +16093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26084B0-3C12-462B-B273-6776CCBE4AD2}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16456,9 +16468,12 @@
       <c r="C25" s="9" t="s">
         <v>308</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -16516,9 +16531,12 @@
       <c r="C29" s="9" t="s">
         <v>312</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -16667,7 +16685,7 @@
       <c r="C39" s="55"/>
       <c r="D39" s="22">
         <f>COUNTA(D5:D38)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E39" s="22">
         <f t="shared" ref="E39:G39" si="1">COUNTA(E5:E38)</f>
@@ -16683,7 +16701,7 @@
       </c>
       <c r="H39" s="23">
         <f>COUNTIF($H$5:$H$38,"X")</f>
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -16717,11 +16735,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>2.9411764705882353E-2</v>
+        <v>8.8235294117647065E-2</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -16730,11 +16748,11 @@
       </c>
       <c r="D45" s="10">
         <f>H39</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>0.97058823529411764</v>
+        <v>0.91176470588235292</v>
       </c>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Carga de libros pdf
Carga de libros pdf para leer
</commit_message>
<xml_diff>
--- a/2020/Directivos-colegio/Coordinacion/listados/20200601 Listado de medios de comunicacion con estudiantes.xlsx
+++ b/2020/Directivos-colegio/Coordinacion/listados/20200601 Listado de medios de comunicacion con estudiantes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\GitHub\liceopatria.github.io\2020\Directivos-colegio\Coordinacion\listados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B412D848-A4CD-44B2-A9CF-1C96CF10C6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AD019B-E764-47B7-B5CD-16B54877B21A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="710" firstSheet="1" activeTab="2" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
+    <workbookView xWindow="2205" yWindow="390" windowWidth="16440" windowHeight="13710" tabRatio="710" firstSheet="3" activeTab="10" xr2:uid="{50E3D567-1B3A-45B1-BFAB-81E44AF5B42C}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="15" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="532">
   <si>
     <t>Codigo</t>
   </si>
@@ -2930,22 +2930,22 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3122,22 +3122,22 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3597,22 +3597,22 @@
                   <c:v>8.8235294117647065E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0303030303030304E-2</c:v>
+                  <c:v>0.93939393939393945</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.87878787878787878</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0303030303030304E-2</c:v>
+                  <c:v>0.21212121212121213</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>0.84848484848484851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3786,22 +3786,22 @@
                   <c:v>0.91176470588235292</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96969696969696972</c:v>
+                  <c:v>6.0606060606060608E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.12121212121212122</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>5.8823529411764705E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.96969696969696972</c:v>
+                  <c:v>0.78787878787878785</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0.15151515151515152</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5659,31 +5659,31 @@
       </c>
       <c r="J5" s="10">
         <f>'10-1'!D43</f>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="K5" s="10">
         <f>'10-2'!D42</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="L5" s="10">
         <f>'10-3'!D43</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="M5" s="10">
         <f>'11-1'!D44</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N5" s="10">
         <f>'11-2'!D43</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O5" s="10">
         <f>'11-3'!D43</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P5" s="33">
         <f t="shared" ref="P5:P8" si="0">AVERAGE(B5:O5)</f>
-        <v>12.357142857142858</v>
+        <v>23</v>
       </c>
       <c r="Q5" s="33">
         <f t="shared" ref="Q5:Q8" si="1">MAX(B5:O5)</f>
@@ -5691,7 +5691,7 @@
       </c>
       <c r="R5" s="33">
         <f t="shared" ref="R5:R8" si="2">MIN(B5:O5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5732,39 +5732,39 @@
       </c>
       <c r="J6" s="10">
         <f>'10-1'!D44</f>
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="K6" s="10">
         <f>'10-2'!D43</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="L6" s="10">
         <f>'10-3'!D44</f>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="M6" s="10">
         <f>'11-1'!D45</f>
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="N6" s="10">
         <f>'11-2'!D44</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="O6" s="10">
         <f>'11-3'!D44</f>
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="P6" s="33">
         <f t="shared" si="0"/>
-        <v>21.714285714285715</v>
+        <v>11.071428571428571</v>
       </c>
       <c r="Q6" s="33">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="R6" s="33">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5805,39 +5805,39 @@
       </c>
       <c r="J7" s="32">
         <f t="shared" si="3"/>
-        <v>3.0303030303030304E-2</v>
+        <v>0.93939393939393945</v>
       </c>
       <c r="K7" s="32">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="L7" s="32">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.87878787878787878</v>
       </c>
       <c r="M7" s="32">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="N7" s="32">
         <f t="shared" si="3"/>
-        <v>3.0303030303030304E-2</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="O7" s="32">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.84848484848484851</v>
       </c>
       <c r="P7" s="34">
         <f t="shared" si="0"/>
-        <v>0.35111089890501651</v>
+        <v>0.67320791953144887</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="1"/>
-        <v>0.875</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="R7" s="34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -5878,39 +5878,39 @@
       </c>
       <c r="J8" s="36">
         <f t="shared" si="4"/>
-        <v>0.96969696969696972</v>
+        <v>6.0606060606060608E-2</v>
       </c>
       <c r="K8" s="36">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="L8" s="36">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="M8" s="36">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="N8" s="36">
         <f t="shared" si="4"/>
-        <v>0.96969696969696972</v>
+        <v>0.78787878787878785</v>
       </c>
       <c r="O8" s="36">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.15151515151515152</v>
       </c>
       <c r="P8" s="37">
         <f t="shared" si="0"/>
-        <v>0.64888910109498354</v>
+        <v>0.32679208046855102</v>
       </c>
       <c r="Q8" s="37">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="R8" s="37">
         <f t="shared" si="2"/>
-        <v>0.125</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
@@ -6259,8 +6259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE5E425-7606-4CA0-91F7-19ECFA2BFA71}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6334,9 +6334,12 @@
       <c r="C5" s="9" t="s">
         <v>322</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H5" s="4" t="str">
         <f>IF(COUNTA(D5:G5)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6349,9 +6352,12 @@
       <c r="C6" s="9" t="s">
         <v>323</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="4" t="str">
         <f t="shared" ref="H6:H37" si="0">IF(COUNTA(D6:G6)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6364,9 +6370,12 @@
       <c r="C7" s="9" t="s">
         <v>324</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6379,9 +6388,12 @@
       <c r="C8" s="9" t="s">
         <v>325</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6394,9 +6406,12 @@
       <c r="C9" s="9" t="s">
         <v>326</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6409,9 +6424,12 @@
       <c r="C10" s="9" t="s">
         <v>327</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -6424,9 +6442,12 @@
       <c r="C11" s="9" t="s">
         <v>328</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -6457,9 +6478,12 @@
       <c r="C13" s="9" t="s">
         <v>330</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6472,9 +6496,12 @@
       <c r="C14" s="9" t="s">
         <v>331</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6487,9 +6514,12 @@
       <c r="C15" s="9" t="s">
         <v>332</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6502,9 +6532,12 @@
       <c r="C16" s="9" t="s">
         <v>333</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -6517,9 +6550,12 @@
       <c r="C17" s="9" t="s">
         <v>334</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -6532,9 +6568,12 @@
       <c r="C18" s="9" t="s">
         <v>335</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -6547,9 +6586,12 @@
       <c r="C19" s="9" t="s">
         <v>336</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -6562,9 +6604,12 @@
       <c r="C20" s="9" t="s">
         <v>337</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -6577,9 +6622,12 @@
       <c r="C21" s="9" t="s">
         <v>338</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -6592,9 +6640,12 @@
       <c r="C22" s="9" t="s">
         <v>339</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -6622,9 +6673,12 @@
       <c r="C24" s="9" t="s">
         <v>341</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -6637,9 +6691,12 @@
       <c r="C25" s="9" t="s">
         <v>342</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -6652,9 +6709,12 @@
       <c r="C26" s="9" t="s">
         <v>343</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -6667,9 +6727,12 @@
       <c r="C27" s="9" t="s">
         <v>344</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -6682,9 +6745,12 @@
       <c r="C28" s="9" t="s">
         <v>345</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -6712,9 +6778,12 @@
       <c r="C30" s="9" t="s">
         <v>347</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -6727,9 +6796,12 @@
       <c r="C31" s="9" t="s">
         <v>348</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -6742,9 +6814,12 @@
       <c r="C32" s="9" t="s">
         <v>349</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -6757,9 +6832,12 @@
       <c r="C33" s="9" t="s">
         <v>350</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -6772,9 +6850,12 @@
       <c r="C34" s="9" t="s">
         <v>351</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -6787,9 +6868,12 @@
       <c r="C35" s="9" t="s">
         <v>352</v>
       </c>
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -6802,9 +6886,12 @@
       <c r="C36" s="9" t="s">
         <v>353</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -6817,9 +6904,12 @@
       <c r="C37" s="9" t="s">
         <v>354</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6830,7 +6920,7 @@
       <c r="C38" s="55"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -6846,7 +6936,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF($H$5:$H$37,"X")</f>
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -6880,11 +6970,11 @@
       </c>
       <c r="D43" s="10">
         <f>D42-D44</f>
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="E43" s="12">
         <f>D43/D42</f>
-        <v>3.0303030303030304E-2</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -6893,11 +6983,11 @@
       </c>
       <c r="D44" s="10">
         <f>H38</f>
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D42</f>
-        <v>0.96969696969696972</v>
+        <v>6.0606060606060608E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6918,11 +7008,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D694D4BB-7FA7-4B24-91F4-C3E54854D28E}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:C36"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6999,9 +7089,12 @@
       <c r="C5" s="9" t="s">
         <v>355</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H5" s="4" t="str">
         <f>IF(COUNTA(D5:G5)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -7014,9 +7107,12 @@
       <c r="C6" s="9" t="s">
         <v>356</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="4" t="str">
         <f t="shared" ref="H6:H36" si="0">IF(COUNTA(D6:G6)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -7059,9 +7155,12 @@
       <c r="C9" s="9" t="s">
         <v>359</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -7074,9 +7173,12 @@
       <c r="C10" s="9" t="s">
         <v>360</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -7089,9 +7191,12 @@
       <c r="C11" s="9" t="s">
         <v>361</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -7104,9 +7209,12 @@
       <c r="C12" s="9" t="s">
         <v>362</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -7119,9 +7227,12 @@
       <c r="C13" s="9" t="s">
         <v>363</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -7149,9 +7260,12 @@
       <c r="C15" s="9" t="s">
         <v>365</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -7164,9 +7278,12 @@
       <c r="C16" s="9" t="s">
         <v>366</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
@@ -7197,9 +7314,12 @@
       <c r="C18" s="9" t="s">
         <v>368</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -7212,9 +7332,12 @@
       <c r="C19" s="9" t="s">
         <v>369</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -7242,9 +7365,12 @@
       <c r="C21" s="9" t="s">
         <v>371</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -7257,9 +7383,12 @@
       <c r="C22" s="9" t="s">
         <v>372</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -7272,9 +7401,12 @@
       <c r="C23" s="9" t="s">
         <v>373</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -7287,9 +7419,12 @@
       <c r="C24" s="9" t="s">
         <v>374</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -7317,9 +7452,12 @@
       <c r="C26" s="9" t="s">
         <v>376</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -7347,9 +7485,12 @@
       <c r="C28" s="9" t="s">
         <v>378</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -7362,9 +7503,12 @@
       <c r="C29" s="9" t="s">
         <v>379</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -7377,9 +7521,12 @@
       <c r="C30" s="9" t="s">
         <v>380</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -7392,9 +7539,12 @@
       <c r="C31" s="9" t="s">
         <v>381</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -7407,9 +7557,12 @@
       <c r="C32" s="9" t="s">
         <v>382</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -7422,9 +7575,12 @@
       <c r="C33" s="9" t="s">
         <v>383</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -7437,9 +7593,12 @@
       <c r="C34" s="9" t="s">
         <v>384</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -7467,9 +7626,12 @@
       <c r="C36" s="9" t="s">
         <v>386</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -7480,23 +7642,23 @@
       <c r="C37" s="55"/>
       <c r="D37" s="22">
         <f>COUNTA(D5:D36)</f>
+        <v>24</v>
+      </c>
+      <c r="E37" s="22">
+        <f t="shared" ref="E37:G37" si="1">COUNTA(E5:E36)</f>
         <v>0</v>
-      </c>
-      <c r="E37" s="22">
-        <f t="shared" ref="E37:G37" si="1">COUNTA(#REF!)</f>
-        <v>1</v>
       </c>
       <c r="F37" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G37" s="22">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="23">
         <f>COUNTIF($H$5:$H$36,"X")</f>
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -7504,9 +7666,7 @@
       <c r="C40" s="18" t="s">
         <v>492</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>493</v>
-      </c>
+      <c r="D40" s="17"/>
       <c r="E40" s="16" t="s">
         <v>494</v>
       </c>
@@ -7530,11 +7690,11 @@
       </c>
       <c r="D42" s="10">
         <f>D41-D43</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E42" s="12">
         <f>D42/D41</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -7543,11 +7703,11 @@
       </c>
       <c r="D43" s="10">
         <f>H37</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E43" s="12">
         <f>D43/D41</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -7568,8 +7728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6AB2A-DF13-43E5-8B37-FC6F541704E3}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7643,9 +7803,12 @@
       <c r="C5" s="9" t="s">
         <v>387</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H5" s="4" t="str">
         <f>IF(COUNTA(D5:G5)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -7658,9 +7821,12 @@
       <c r="C6" s="9" t="s">
         <v>388</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="4" t="str">
         <f t="shared" ref="H6:H37" si="0">IF(COUNTA(D6:G6)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -7673,9 +7839,12 @@
       <c r="C7" s="9" t="s">
         <v>389</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7703,9 +7872,12 @@
       <c r="C9" s="9" t="s">
         <v>391</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -7718,9 +7890,12 @@
       <c r="C10" s="9" t="s">
         <v>392</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7733,9 +7908,12 @@
       <c r="C11" s="9" t="s">
         <v>393</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7748,9 +7926,12 @@
       <c r="C12" s="9" t="s">
         <v>394</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7763,9 +7944,12 @@
       <c r="C13" s="9" t="s">
         <v>395</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -7778,9 +7962,12 @@
       <c r="C14" s="9" t="s">
         <v>396</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -7793,9 +7980,12 @@
       <c r="C15" s="9" t="s">
         <v>397</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -7808,9 +7998,12 @@
       <c r="C16" s="9" t="s">
         <v>398</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -7823,9 +8016,12 @@
       <c r="C17" s="9" t="s">
         <v>399</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7838,9 +8034,12 @@
       <c r="C18" s="9" t="s">
         <v>400</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7853,9 +8052,12 @@
       <c r="C19" s="9" t="s">
         <v>401</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -7868,9 +8070,12 @@
       <c r="C20" s="9" t="s">
         <v>402</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -7883,9 +8088,12 @@
       <c r="C21" s="9" t="s">
         <v>403</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -7898,9 +8106,12 @@
       <c r="C22" s="9" t="s">
         <v>404</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -7943,9 +8154,12 @@
       <c r="C25" s="9" t="s">
         <v>407</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -7973,9 +8187,12 @@
       <c r="C27" s="9" t="s">
         <v>409</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -7988,9 +8205,12 @@
       <c r="C28" s="9" t="s">
         <v>410</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -8003,9 +8223,12 @@
       <c r="C29" s="9" t="s">
         <v>411</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -8018,9 +8241,12 @@
       <c r="C30" s="9" t="s">
         <v>412</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -8033,9 +8259,12 @@
       <c r="C31" s="9" t="s">
         <v>413</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -8048,9 +8277,12 @@
       <c r="C32" s="9" t="s">
         <v>414</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -8063,9 +8295,12 @@
       <c r="C33" s="9" t="s">
         <v>415</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -8078,9 +8313,12 @@
       <c r="C34" s="9" t="s">
         <v>416</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -8093,9 +8331,12 @@
       <c r="C35" s="9" t="s">
         <v>417</v>
       </c>
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -8108,9 +8349,12 @@
       <c r="C36" s="9" t="s">
         <v>418</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -8123,9 +8367,12 @@
       <c r="C37" s="9" t="s">
         <v>419</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8136,7 +8383,7 @@
       <c r="C38" s="55"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -8152,7 +8399,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -8186,11 +8433,11 @@
       </c>
       <c r="D43" s="10">
         <f>D42-D44</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E43" s="12">
         <f>D43/D42</f>
-        <v>0</v>
+        <v>0.87878787878787878</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -8199,11 +8446,11 @@
       </c>
       <c r="D44" s="10">
         <f>H38</f>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D42</f>
-        <v>1</v>
+        <v>0.12121212121212122</v>
       </c>
     </row>
   </sheetData>
@@ -8299,9 +8546,12 @@
       <c r="C5" s="9" t="s">
         <v>420</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H5" s="4" t="str">
         <f>IF(COUNTA(D5:G5)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -8314,9 +8564,12 @@
       <c r="C6" s="9" t="s">
         <v>421</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="4" t="str">
         <f t="shared" ref="H6:H38" si="0">IF(COUNTA(D6:G6)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -8329,9 +8582,12 @@
       <c r="C7" s="9" t="s">
         <v>422</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -8344,9 +8600,12 @@
       <c r="C8" s="9" t="s">
         <v>423</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -8359,9 +8618,12 @@
       <c r="C9" s="9" t="s">
         <v>424</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -8374,9 +8636,12 @@
       <c r="C10" s="9" t="s">
         <v>425</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -8389,9 +8654,12 @@
       <c r="C11" s="9" t="s">
         <v>426</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -8404,9 +8672,12 @@
       <c r="C12" s="9" t="s">
         <v>427</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -8419,9 +8690,12 @@
       <c r="C13" s="9" t="s">
         <v>428</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -8434,9 +8708,12 @@
       <c r="C14" s="9" t="s">
         <v>429</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -8449,9 +8726,12 @@
       <c r="C15" s="9" t="s">
         <v>430</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -8464,9 +8744,12 @@
       <c r="C16" s="9" t="s">
         <v>431</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -8479,9 +8762,12 @@
       <c r="C17" s="9" t="s">
         <v>432</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -8509,9 +8795,12 @@
       <c r="C19" s="9" t="s">
         <v>434</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -8524,9 +8813,12 @@
       <c r="C20" s="9" t="s">
         <v>435</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -8539,9 +8831,12 @@
       <c r="C21" s="9" t="s">
         <v>436</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -8554,9 +8849,12 @@
       <c r="C22" s="9" t="s">
         <v>437</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -8569,9 +8867,12 @@
       <c r="C23" s="9" t="s">
         <v>438</v>
       </c>
+      <c r="D23" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -8584,9 +8885,12 @@
       <c r="C24" s="9" t="s">
         <v>439</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -8599,9 +8903,12 @@
       <c r="C25" s="9" t="s">
         <v>440</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -8614,9 +8921,12 @@
       <c r="C26" s="9" t="s">
         <v>441</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -8629,9 +8939,12 @@
       <c r="C27" s="9" t="s">
         <v>442</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -8644,9 +8957,12 @@
       <c r="C28" s="9" t="s">
         <v>443</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -8659,9 +8975,12 @@
       <c r="C29" s="9" t="s">
         <v>444</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -8689,9 +9008,12 @@
       <c r="C31" s="9" t="s">
         <v>446</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -8704,9 +9026,12 @@
       <c r="C32" s="9" t="s">
         <v>447</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -8719,9 +9044,12 @@
       <c r="C33" s="9" t="s">
         <v>448</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -8734,9 +9062,12 @@
       <c r="C34" s="9" t="s">
         <v>449</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -8749,9 +9080,12 @@
       <c r="C35" s="9" t="s">
         <v>450</v>
       </c>
+      <c r="D35" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -8764,9 +9098,12 @@
       <c r="C36" s="9" t="s">
         <v>451</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -8779,9 +9116,12 @@
       <c r="C37" s="9" t="s">
         <v>452</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -8794,9 +9134,12 @@
       <c r="C38" s="9" t="s">
         <v>453</v>
       </c>
+      <c r="D38" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8807,7 +9150,7 @@
       <c r="C39" s="55"/>
       <c r="D39" s="22">
         <f>COUNTA(D5:D38)</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E39" s="22">
         <f t="shared" ref="E39:G39" si="1">COUNTA(E5:E38)</f>
@@ -8823,7 +9166,7 @@
       </c>
       <c r="H39" s="23">
         <f>COUNTIF(H5:H38,"X")</f>
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -8857,11 +9200,11 @@
       </c>
       <c r="D44" s="10">
         <f>D43-D45</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D43</f>
-        <v>0</v>
+        <v>0.94117647058823528</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -8870,11 +9213,11 @@
       </c>
       <c r="D45" s="10">
         <f>H39</f>
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E45" s="12">
         <f>D45/D43</f>
-        <v>1</v>
+        <v>5.8823529411764705E-2</v>
       </c>
     </row>
   </sheetData>
@@ -8896,7 +9239,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D37"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9042,10 +9385,12 @@
       <c r="C9" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -9122,10 +9467,12 @@
       <c r="C14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -9138,10 +9485,12 @@
       <c r="C15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -9170,10 +9519,12 @@
       <c r="C17" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -9234,10 +9585,12 @@
       <c r="C21" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -9298,10 +9651,12 @@
       <c r="C25" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -9507,7 +9862,7 @@
       <c r="C38" s="55"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -9523,7 +9878,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -9557,11 +9912,11 @@
       </c>
       <c r="D43" s="10">
         <f>D42-D44</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E43" s="12">
         <f>D43/D42</f>
-        <v>3.0303030303030304E-2</v>
+        <v>0.21212121212121213</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -9570,11 +9925,11 @@
       </c>
       <c r="D44" s="10">
         <f>H38</f>
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E44" s="12">
         <f>D44/D42</f>
-        <v>0.96969696969696972</v>
+        <v>0.78787878787878785</v>
       </c>
     </row>
   </sheetData>
@@ -9595,8 +9950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D56A688-FE73-4566-841A-31D529165F68}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D37"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9670,9 +10025,12 @@
       <c r="C5" s="9" t="s">
         <v>454</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H5" s="4" t="str">
         <f>IF(COUNTA(D5:G5)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -9685,9 +10043,12 @@
       <c r="C6" s="9" t="s">
         <v>455</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="4" t="str">
         <f t="shared" ref="H6:H37" si="0">IF(COUNTA(D6:G6)=0,"X","")</f>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -9700,9 +10061,12 @@
       <c r="C7" s="9" t="s">
         <v>456</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -9715,9 +10079,12 @@
       <c r="C8" s="9" t="s">
         <v>457</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -9730,9 +10097,12 @@
       <c r="C9" s="9" t="s">
         <v>458</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -9760,9 +10130,12 @@
       <c r="C11" s="9" t="s">
         <v>460</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -9775,9 +10148,12 @@
       <c r="C12" s="9" t="s">
         <v>461</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -9790,9 +10166,12 @@
       <c r="C13" s="9" t="s">
         <v>462</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -9805,9 +10184,12 @@
       <c r="C14" s="9" t="s">
         <v>463</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -9820,9 +10202,12 @@
       <c r="C15" s="9" t="s">
         <v>464</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -9835,9 +10220,12 @@
       <c r="C16" s="9" t="s">
         <v>465</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -9850,9 +10238,12 @@
       <c r="C17" s="9" t="s">
         <v>466</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -9865,9 +10256,12 @@
       <c r="C18" s="9" t="s">
         <v>467</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -9895,9 +10289,12 @@
       <c r="C20" s="9" t="s">
         <v>469</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -9910,9 +10307,12 @@
       <c r="C21" s="9" t="s">
         <v>470</v>
       </c>
+      <c r="D21" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -9925,9 +10325,12 @@
       <c r="C22" s="9" t="s">
         <v>471</v>
       </c>
+      <c r="D22" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -9955,9 +10358,12 @@
       <c r="C24" s="9" t="s">
         <v>473</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -9970,9 +10376,12 @@
       <c r="C25" s="9" t="s">
         <v>474</v>
       </c>
+      <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -9985,9 +10394,12 @@
       <c r="C26" s="9" t="s">
         <v>475</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -10000,9 +10412,12 @@
       <c r="C27" s="9" t="s">
         <v>476</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -10015,9 +10430,12 @@
       <c r="C28" s="9" t="s">
         <v>477</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -10030,9 +10448,12 @@
       <c r="C29" s="9" t="s">
         <v>478</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -10045,9 +10466,12 @@
       <c r="C30" s="9" t="s">
         <v>479</v>
       </c>
+      <c r="D30" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -10060,9 +10484,12 @@
       <c r="C31" s="9" t="s">
         <v>480</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -10075,9 +10502,12 @@
       <c r="C32" s="9" t="s">
         <v>481</v>
       </c>
+      <c r="D32" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -10090,9 +10520,12 @@
       <c r="C33" s="9" t="s">
         <v>482</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -10105,9 +10538,12 @@
       <c r="C34" s="9" t="s">
         <v>483</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -10150,9 +10586,12 @@
       <c r="C37" s="9" t="s">
         <v>486</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="H37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v/>
       </c>
     </row>
     <row r="38" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -10163,7 +10602,7 @@
       <c r="C38" s="55"/>
       <c r="D38" s="22">
         <f>COUNTA(D5:D37)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:G38" si="1">COUNTA(E5:E37)</f>
@@ -10179,7 +10618,7 @@
       </c>
       <c r="H38" s="23">
         <f>COUNTIF(H5:H37,"X")</f>
-        <v>33</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -10212,7 +10651,7 @@
       </c>
       <c r="D43" s="10">
         <f>D42-D44</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E43" s="12">
         <v>0.8529411764705882</v>
@@ -10224,7 +10663,7 @@
       </c>
       <c r="D44" s="10">
         <f>H38</f>
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E44" s="12">
         <v>0.14705882352941177</v>
@@ -11233,8 +11672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8FFEA4-FAE9-4E98-A7DA-1A249C6193F4}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>